<commit_message>
Added code to List unallocated Requirement and Resource
</commit_message>
<xml_diff>
--- a/Resource Allocation Sheet - Original.xlsx
+++ b/Resource Allocation Sheet - Original.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -602,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2">
-        <v>42205</v>
+        <v>42180</v>
       </c>
       <c r="D16" s="2">
         <v>42237</v>
@@ -905,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2">
-        <v>42205</v>
+        <v>42180</v>
       </c>
       <c r="D17" s="2">
         <v>42237</v>
@@ -922,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2">
-        <v>42205</v>
+        <v>42180</v>
       </c>
       <c r="D18" s="2">
         <v>42237</v>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2">
-        <v>42205</v>
+        <v>42180</v>
       </c>
       <c r="D19" s="2">
         <v>42237</v>
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2">
-        <v>42205</v>
+        <v>42180</v>
       </c>
       <c r="D20" s="2">
         <v>42237</v>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="2">
-        <v>42205</v>
+        <v>42180</v>
       </c>
       <c r="D21" s="2">
         <v>42237</v>
@@ -990,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>42193</v>
+        <v>42180</v>
       </c>
       <c r="D22" s="2">
         <v>42237</v>
@@ -1007,7 +1007,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2">
-        <v>42193</v>
+        <v>42180</v>
       </c>
       <c r="D23" s="2">
         <v>42237</v>
@@ -1024,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="2">
-        <v>42193</v>
+        <v>42180</v>
       </c>
       <c r="D24" s="2">
         <v>42237</v>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>42193</v>
+        <v>42180</v>
       </c>
       <c r="D25" s="2">
         <v>42237</v>
@@ -1058,7 +1058,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2">
-        <v>42193</v>
+        <v>42180</v>
       </c>
       <c r="D26" s="2">
         <v>42237</v>
@@ -1075,7 +1075,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="2">
-        <v>42193</v>
+        <v>42180</v>
       </c>
       <c r="D27" s="2">
         <v>42237</v>
@@ -1094,7 +1094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Code Added to find better allocation either by Resource or By Available Days.
</commit_message>
<xml_diff>
--- a/Resource Allocation Sheet - Original.xlsx
+++ b/Resource Allocation Sheet - Original.xlsx
@@ -602,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,7 +613,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>42180</v>
+        <v>42237</v>
       </c>
       <c r="D25" s="2">
         <v>42237</v>
@@ -1075,7 +1075,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="2">
-        <v>42180</v>
+        <v>42237</v>
       </c>
       <c r="D27" s="2">
         <v>42237</v>
@@ -1095,7 +1095,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>